<commit_message>
Added code to extract features from x-ray images having pneumonia disease
</commit_message>
<xml_diff>
--- a/normal.xlsx
+++ b/normal.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1342"/>
+  <dimension ref="A1:D1342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,15 +433,10 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Mode</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>Variance</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Std</t>
         </is>

</xml_diff>